<commit_message>
Parts purchase and Job creation job updated from Repair
</commit_message>
<xml_diff>
--- a/Buzzworld_InternalPortal/tcfile.xlsx
+++ b/Buzzworld_InternalPortal/tcfile.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="138">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -93,12 +93,6 @@
   </si>
   <si>
     <t>Failed</t>
-  </si>
-  <si>
-    <t>2023-10-11 15:05:03</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>2023-10-11 14:30:37</t>
@@ -293,6 +287,169 @@
   </si>
   <si>
     <t>2023-10-11 14:47:02</t>
+  </si>
+  <si>
+    <t>PERMNS_035_Verify_Pricing_Permission_As_None</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:43:40</t>
+  </si>
+  <si>
+    <t>PERMNS_036_Verify_Discount Codes_Permission_As_None</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:44:13</t>
+  </si>
+  <si>
+    <t>PERMNS_037_Verify_Non Standard Pricing_Permission_As_None</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:44:46</t>
+  </si>
+  <si>
+    <t>PERMNS_038_Verify_Export_Permission_As_Yes_In_Pricing</t>
+  </si>
+  <si>
+    <t>Centrifuge
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>Top displayed text is Centrifuge
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:45:22</t>
+  </si>
+  <si>
+    <t>PERMNS_039_Verify_Export_Permission_As_NoIn_Pricing</t>
+  </si>
+  <si>
+    <t>Centrifuge
+Export
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>Top displayed text is Centrifuge
+Export
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:45:58</t>
+  </si>
+  <si>
+    <t>PERMNS_040_Verify_Import_Permission_As_Yes_In_Pricing</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:46:35</t>
+  </si>
+  <si>
+    <t>PERMNS_041_Verify_Import_Permission_As_No_In_Pricing</t>
+  </si>
+  <si>
+    <t>Centrifuge
+Import
+Export
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>Top displayed text is Centrifuge
+Import
+Export
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:47:11</t>
+  </si>
+  <si>
+    <t>PERMNS_042_Verify_Export_Permission_As_Yes_In_Discount Codes</t>
+  </si>
+  <si>
+    <t>Centrifuge
+Multi Edit
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>Top displayed text is Centrifuge
+Multi Edit
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:47:48</t>
+  </si>
+  <si>
+    <t>PERMNS_043_Verify_Export_Permission_As_No_In_Discount Codes</t>
+  </si>
+  <si>
+    <t>Centrifuge
+Multi Edit
+Export
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>Top displayed text is Centrifuge
+Multi Edit
+Export
+Filters
+Add</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:48:24</t>
+  </si>
+  <si>
+    <t>PERMNS_044_Verify_Export_Permission_As_Yes_In_Non Standard Pricing</t>
+  </si>
+  <si>
+    <t>Pricing Rule Configurator
+Export</t>
+  </si>
+  <si>
+    <t>Top displayed text is Pricing Rule Configurator
+Export</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:49:08</t>
+  </si>
+  <si>
+    <t>PERMNS_045_Verify_Export_Permission_As_No_In_Non Standard Pricing</t>
+  </si>
+  <si>
+    <t>Pricing Rule Configurator</t>
+  </si>
+  <si>
+    <t>Top displayed text is Pricing Rule Configurator</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:49:51</t>
+  </si>
+  <si>
+    <t>PERMNS_046_Verify_Pricing_Permission_As_View</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:50:25</t>
+  </si>
+  <si>
+    <t>PERMNS_047_Verify_Discount Codes_Permission_As_View</t>
+  </si>
+  <si>
+    <t>2023-10-11 16:50:58</t>
+  </si>
+  <si>
+    <t>PERMNS_048_Verify_Non Standard Pricing_Permission_As_View</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2023-10-11 16:51:30</t>
   </si>
   <si>
     <t>PERMNS_094_Verify_Product Category_Permission_As_View</t>
@@ -368,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="G2" activePane="bottomRight" xSplit="6.0"/>
@@ -567,24 +724,24 @@
         <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
         <v>29</v>
@@ -716,13 +873,13 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
         <v>41</v>
@@ -739,13 +896,13 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
         <v>43</v>
@@ -805,10 +962,10 @@
         <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>10</v>
@@ -817,7 +974,7 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
         <v>13</v>
@@ -825,13 +982,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
         <v>50</v>
-      </c>
-      <c r="B20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
@@ -851,19 +1008,19 @@
         <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -871,13 +1028,13 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -897,10 +1054,10 @@
         <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s">
         <v>10</v>
@@ -920,10 +1077,10 @@
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>10</v>
@@ -932,7 +1089,7 @@
         <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G24" t="s">
         <v>13</v>
@@ -940,13 +1097,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
         <v>10</v>
@@ -966,10 +1123,10 @@
         <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
         <v>10</v>
@@ -989,10 +1146,10 @@
         <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
@@ -1012,10 +1169,10 @@
         <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
         <v>10</v>
@@ -1024,7 +1181,7 @@
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G28" t="s">
         <v>13</v>
@@ -1032,13 +1189,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
         <v>10</v>
@@ -1058,10 +1215,10 @@
         <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D30" t="s">
         <v>10</v>
@@ -1081,10 +1238,10 @@
         <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
         <v>10</v>
@@ -1104,19 +1261,19 @@
         <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
         <v>10</v>
       </c>
       <c r="E32" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G32" t="s">
         <v>13</v>
@@ -1124,13 +1281,13 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
         <v>10</v>
@@ -1139,7 +1296,7 @@
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G33" t="s">
         <v>13</v>
@@ -1147,13 +1304,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
         <v>10</v>
@@ -1173,10 +1330,10 @@
         <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" t="s">
         <v>10</v>
@@ -1196,10 +1353,10 @@
         <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="D36" t="s">
         <v>10</v>
@@ -1219,16 +1376,16 @@
         <v>93</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F37" t="s">
         <v>94</v>
@@ -1257,6 +1414,305 @@
         <v>96</v>
       </c>
       <c r="G38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>97</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="B40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" t="s">
+        <v>104</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F41" t="s">
+        <v>106</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>107</v>
+      </c>
+      <c r="B42" t="s">
+        <v>108</v>
+      </c>
+      <c r="C42" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43" t="s">
+        <v>114</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>118</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>122</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
+        <v>126</v>
+      </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" t="s">
+        <v>130</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>133</v>
+      </c>
+      <c r="G49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50" t="s">
+        <v>135</v>
+      </c>
+      <c r="G50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>136</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" t="s">
+        <v>137</v>
+      </c>
+      <c r="G51" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>